<commit_message>
updated numero to cantidad
</commit_message>
<xml_diff>
--- a/resources/assets/excel/ingresarexcel.xlsx
+++ b/resources/assets/excel/ingresarexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\lsapp3\resources\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBBB629-2B3A-4F8C-886F-1AA42E0D9149}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91183621-6A41-4E0D-9440-B03B5653FA66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="786" firstSheet="3" activeTab="6" xr2:uid="{36B60C1C-FBE5-4F8D-81CA-193DEC5AF82E}"/>
+    <workbookView xWindow="4284" yWindow="1848" windowWidth="17280" windowHeight="9072" tabRatio="786" firstSheet="3" activeTab="6" xr2:uid="{36B60C1C-FBE5-4F8D-81CA-193DEC5AF82E}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICION" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="166">
   <si>
     <t>fecha</t>
   </si>
@@ -529,6 +529,18 @@
   </si>
   <si>
     <t>Portificus grandotus</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>0-30 m de diámetro</t>
+  </si>
+  <si>
+    <t>&gt;30 m de diámetro</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -858,7 +870,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1017,6 +1029,9 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3215,27 +3230,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E68EAA1-00AC-4C2B-AC96-2ADF2DD2B9C2}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" style="10" customWidth="1"/>
-    <col min="2" max="3" width="24" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="10" customWidth="1"/>
-    <col min="6" max="7" width="16.88671875" style="10" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="10"/>
-    <col min="11" max="11" width="16.6640625" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="10"/>
+    <col min="2" max="4" width="24" style="10" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="10" customWidth="1"/>
+    <col min="7" max="8" width="16.88671875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="10"/>
+    <col min="12" max="12" width="16.6640625" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
@@ -3246,31 +3261,34 @@
         <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>38</v>
       </c>
@@ -3280,14 +3298,14 @@
       <c r="C2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>45</v>
@@ -3304,8 +3322,11 @@
       <c r="K2" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>39</v>
       </c>
@@ -3315,32 +3336,35 @@
       <c r="C3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="12">
-        <v>4</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="D3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
@@ -3350,14 +3374,14 @@
       <c r="C4" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="D4" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>152</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>45</v>
@@ -3366,245 +3390,269 @@
         <v>45</v>
       </c>
       <c r="I4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>